<commit_message>
update naming and add etf list
</commit_message>
<xml_diff>
--- a/US_StrongBuy_Scan_20251110.xlsx
+++ b/US_StrongBuy_Scan_20251110.xlsx
@@ -7,9 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="⭐Strong Buy" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="✅Buy" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Industry Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stock ⭐Strong Buy" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stock ✅Buy" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ETF ⭐Strong Buy" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ETF ✅Buy" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Industry Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ETF Overview" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,35 +441,40 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>股票代码</t>
+          <t>类别</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>涨跌幅 %</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>成交量/均量比</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>策略评分</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>评级</t>
         </is>
@@ -475,25 +483,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>GOOGL</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>290.1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>4.04</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>71.59999999999999</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.88</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>90</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>⭐ 强买入</t>
         </is>
@@ -502,25 +515,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>CRWD</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>557.53</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>3.28</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.96</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>90</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>⭐ 强买入</t>
         </is>
@@ -537,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,35 +566,40 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>股票代码</t>
+          <t>类别</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>涨跌幅 %</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>成交量/均量比</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>策略评分</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>评级</t>
         </is>
@@ -585,25 +608,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>CSCO</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>72.09</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>1.44</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>56.1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1.29</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>80</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -612,25 +640,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>MU</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>253.3</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>6.46</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1.21</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>80</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -639,25 +672,30 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>AAPL</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>269.43</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.36</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>64.90000000000001</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.83</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>70</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -666,25 +704,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>NVDA</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>199.05</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>5.79</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>57.5</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>1.05</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>70</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -693,25 +736,30 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>LITE</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>259.89</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>8.24</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>77.40000000000001</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.62</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>70</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -723,6 +771,192 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>类别</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>涨跌幅 %</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>成交量/均量比</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>策略评分</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>评级</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>类别</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>涨跌幅 %</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>成交量/均量比</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>策略评分</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>评级</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>681.4400000000001</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="E2" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G2" t="n">
+        <v>70</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>✅ 买入</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>QQQ</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>623.23</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="E3" t="n">
+        <v>56</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="G3" t="n">
+        <v>70</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>✅ 买入</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -760,10 +994,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>74</v>
+        <v>72.85714285714286</v>
       </c>
     </row>
     <row r="3">
@@ -777,6 +1011,179 @@
       </c>
       <c r="C3" t="n">
         <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>站上MA20</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>站上MA50</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MACD&gt;Signal</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MA20上升</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MA50上升</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>与MA20偏离%</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>与MA50偏离%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>681.4400000000001</v>
+      </c>
+      <c r="C2" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>QQQ</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>623.23</v>
+      </c>
+      <c r="C3" t="n">
+        <v>56</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IWM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>244.03</v>
+      </c>
+      <c r="C4" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.71</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add shorting, more etf list
</commit_message>
<xml_diff>
--- a/US_StrongBuy_Scan_20251110.xlsx
+++ b/US_StrongBuy_Scan_20251110.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stock ⭐Strong Buy" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stock ✅Buy" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ETF ⭐Strong Buy" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ETF ✅Buy" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Industry Summary" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ETF Overview" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Stock ⭐Strong Buy" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Stock ✅Buy" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Stock 🔻Strong Short" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Stock ⚠️Short" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ETF ⭐Strong Buy" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ETF ✅Buy" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ETF 🔻Strong Short" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ETF ⚠️Short" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Industry Summary" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="ETF Overview" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,35 +450,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>涨跌幅 %</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>成交量/均量比</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>策略评分</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>评级</t>
         </is>
@@ -488,25 +497,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GOOGL</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>290.1</v>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CRWD</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>4.04</v>
+        <v>557.53</v>
       </c>
       <c r="E2" t="n">
-        <v>71.59999999999999</v>
+        <v>3.28</v>
       </c>
       <c r="F2" t="n">
-        <v>0.88</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="G2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H2" t="n">
         <v>90</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>⭐ 强买入</t>
         </is>
@@ -520,28 +534,285 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CRWD</t>
-        </is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>72.09</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="F3" t="n">
+        <v>56.1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H3" t="n">
+        <v>90</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>⭐ 强买入</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>290.1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="F4" t="n">
+        <v>71.59999999999999</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="H4" t="n">
+        <v>90</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>⭐ 强买入</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>站上MA20</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>站上MA50</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MACD&gt;Signal</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MA20上升</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MA50上升</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>与MA20偏离%</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>与MA50偏离%</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>OBV&gt;MA20</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>OBV上升</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>与OBV_MA20偏离%</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>681.4400000000001</v>
+      </c>
+      <c r="C2" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>64.15000000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>QQQ</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>623.23</v>
       </c>
       <c r="C3" t="n">
-        <v>557.53</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3.28</v>
-      </c>
-      <c r="E3" t="n">
-        <v>67.59999999999999</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="G3" t="n">
-        <v>90</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>⭐ 强买入</t>
-        </is>
+        <v>56</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>13.59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IWM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>244.03</v>
+      </c>
+      <c r="C4" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.71</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-4.92</v>
       </c>
     </row>
   </sheetData>
@@ -555,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,35 +842,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>涨跌幅 %</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>成交量/均量比</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>策略评分</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>评级</t>
         </is>
@@ -613,25 +889,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CSCO</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>72.09</v>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>1.44</v>
+        <v>269.43</v>
       </c>
       <c r="E2" t="n">
-        <v>56.1</v>
+        <v>0.36</v>
       </c>
       <c r="F2" t="n">
-        <v>1.29</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="G2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="H2" t="n">
         <v>80</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -645,25 +926,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>MU</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>253.3</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>6.46</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1.21</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>80</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -677,25 +963,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AAPL</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>269.43</v>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>0.36</v>
+        <v>199.05</v>
       </c>
       <c r="E4" t="n">
-        <v>64.90000000000001</v>
+        <v>5.79</v>
       </c>
       <c r="F4" t="n">
-        <v>0.83</v>
+        <v>57.5</v>
       </c>
       <c r="G4" t="n">
-        <v>70</v>
-      </c>
-      <c r="H4" t="inlineStr">
+        <v>1.05</v>
+      </c>
+      <c r="H4" t="n">
+        <v>80</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -709,57 +1000,30 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>199.05</v>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
       </c>
       <c r="D5" t="n">
-        <v>5.79</v>
+        <v>259.89</v>
       </c>
       <c r="E5" t="n">
-        <v>57.5</v>
+        <v>8.24</v>
       </c>
       <c r="F5" t="n">
-        <v>1.05</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="G5" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H5" t="n">
         <v>70</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>✅ 买入</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>股票</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LITE</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>259.89</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8.24</v>
-      </c>
-      <c r="E6" t="n">
-        <v>77.40000000000001</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="G6" t="n">
-        <v>70</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>✅ 买入</t>
         </is>
@@ -776,7 +1040,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -792,35 +1056,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>涨跌幅 %</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>成交量/均量比</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>策略评分</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>评级</t>
         </is>
@@ -837,7 +1106,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,35 +1122,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>涨跌幅 %</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>成交量/均量比</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>策略评分</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>评级</t>
         </is>
@@ -890,64 +1164,185 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>股票</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SPY</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>681.4400000000001</v>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>1.56</v>
+        <v>631.76</v>
       </c>
       <c r="E2" t="n">
-        <v>57.7</v>
+        <v>1.62</v>
       </c>
       <c r="F2" t="n">
-        <v>0.97</v>
+        <v>30.6</v>
       </c>
       <c r="G2" t="n">
-        <v>70</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>✅ 买入</t>
+        <v>0.89</v>
+      </c>
+      <c r="H2" t="n">
+        <v>80</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>⚠️ 做空</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>股票</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>QQQ</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>623.23</v>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>2.21</v>
+        <v>506</v>
       </c>
       <c r="E3" t="n">
-        <v>56</v>
+        <v>1.85</v>
       </c>
       <c r="F3" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="H3" t="n">
+        <v>80</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>⚠️ 做空</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>FCX</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>40.95</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="F4" t="n">
+        <v>49.7</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.9399999999999999</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H4" t="n">
         <v>70</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>✅ 买入</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>⚠️ 做空</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HIMS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>41.05</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F5" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>70</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>⚠️ 做空</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>股票</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>40.19</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="F6" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="H6" t="n">
+        <v>70</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>⚠️ 做空</t>
         </is>
       </c>
     </row>
@@ -962,7 +1357,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,44 +1368,48 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>类别</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>涨跌幅 %</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>成交量/均量比</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>策略评分</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>评级</t>
         </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>count</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>✅ 买入</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>7</v>
-      </c>
-      <c r="C2" t="n">
-        <v>72.85714285714286</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>⭐ 强买入</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1024,7 +1423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1035,155 +1434,329 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>类别</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>收盘价</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>涨跌幅 %</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RSI</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>站上MA20</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>站上MA50</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MACD&gt;Signal</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>MA20上升</t>
+          <t>成交量/均量比</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>MA50上升</t>
+          <t>策略评分</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>与MA20偏离%</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>与MA50偏离%</t>
+          <t>评级</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SPY</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>681.4400000000001</v>
-      </c>
-      <c r="C2" t="n">
-        <v>57.7</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.34</v>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>QQQ</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>623.23</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="F2" t="n">
+        <v>56</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>80</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>✅ 买入</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>QQQ</t>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>681.4400000000001</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="F3" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="H3" t="n">
+        <v>80</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>✅ 买入</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>类别</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>涨跌幅 %</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>成交量/均量比</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>策略评分</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>评级</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>类别</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>代码</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>收盘价</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>涨跌幅 %</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>成交量/均量比</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>策略评分</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>评级</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>评级</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>⚠️ 做空</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>✅ 买入</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>623.23</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>56</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="J3" t="n">
-        <v>3.46</v>
+        <v>78.33333333333333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IWM</t>
+          <t>⭐ 强买入</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>244.03</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>49.9</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>-0.71</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.47</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>